<commit_message>
update hydra project v2.0 and update cmscript
</commit_message>
<xml_diff>
--- a/hydra_tas/TimeSheet.xlsx
+++ b/hydra_tas/TimeSheet.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2445" yWindow="2145" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="dictionary" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$J$2</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="79">
   <si>
     <t>Active Code Category</t>
   </si>
@@ -153,23 +153,293 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Quilty Check</t>
-  </si>
-  <si>
     <t>QA Audit</t>
   </si>
   <si>
     <t>Mini Assessment</t>
   </si>
   <si>
-    <t>deal with email</t>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mandontory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">input : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Time Sheet for … --&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Cost Centre</t>
+  </si>
+  <si>
+    <t>ODC:Falcon</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> *  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Attentions:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1. Make sure "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bleum"</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> at the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bottom</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Cost Centre </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Column;  2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Double check</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> your TAS after scripts!!</t>
+    </r>
+  </si>
+  <si>
+    <t>Rqmt</t>
+  </si>
+  <si>
+    <t>Review Req.</t>
+  </si>
+  <si>
+    <t>OP001</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Conferencer call and daily Meeting</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Domain Training</t>
+  </si>
+  <si>
+    <t>Benefits</t>
+  </si>
+  <si>
+    <t>Paid Leave</t>
+  </si>
+  <si>
+    <t>Paid off leave</t>
+  </si>
+  <si>
+    <t>Public Holidays</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Eng Training</t>
+  </si>
+  <si>
+    <t>Quilty Check and Quiz</t>
+  </si>
+  <si>
+    <t>T113</t>
+  </si>
+  <si>
+    <t>QA Call</t>
+  </si>
+  <si>
+    <t>1FB Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review Oqs and attend group review </t>
+  </si>
+  <si>
+    <t>This Week</t>
+  </si>
+  <si>
+    <t>Tech Training</t>
+  </si>
+  <si>
+    <t>OP Product</t>
+  </si>
+  <si>
+    <t>Set up and maintain CI/bw env</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,13 +455,95 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -203,17 +555,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,101 +878,607 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1153</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="I4">
+        <v>0.5</v>
+      </c>
+      <c r="J4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>1154</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>1171</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>1177</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>0.1</v>
+      </c>
+      <c r="I7">
+        <v>0.1</v>
+      </c>
+      <c r="J7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <v>1166</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>1166</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>9011</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+      <c r="G10">
+        <v>0.5</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+      <c r="I10">
+        <v>0.5</v>
+      </c>
+      <c r="J10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>9011</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12">
+        <v>4462</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>2.5</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>1153</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2">
-        <v>0.5</v>
-      </c>
-      <c r="G2">
-        <v>0.5</v>
-      </c>
-      <c r="H2">
-        <v>0.5</v>
-      </c>
-      <c r="I2">
-        <v>0.5</v>
-      </c>
-      <c r="J2">
-        <v>0.5</v>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>9011</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <v>9023</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J2"/>
+  <autoFilter ref="A2:J2"/>
   <dataConsolidate/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
-      <formula1>"Admin&amp;HR,Quality,SCM,Test,Training"</formula1>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:J1"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
+      <formula1>"Last Week,This Week,Next Week"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
-      <formula1>"Email,TAS,Resource Mgt,Technical,Manage change,Setup Env.,Draft Spec.,Tech. Improve,Resource Mgt,Reimburse,QA Pcm,QA Audit,Build&amp;Install"</formula1>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="double_chk" error="Please double check, maybe NOT iin Hydra List" sqref="C3:C1048576">
+      <formula1>"Email,TAS,Resource Mgt,Reimburse,Tech. Improve,Technical,Manage change,Review Req.,Setup Env.,Build&amp;Install,Draft Spec.,Manage change,Meeting,Domain,QA Pcm,QA Audit,Paid Leave,Public Holidays,English"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
-      <formula1>"1FB ODC,Affinity Product,CS-Maintenance,Bleum"</formula1>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="double_chk" error="Please double check, maybe NOT iin Hydra List" sqref="B3:B1048576">
+      <formula1>"Admin&amp;HR,Quality,SCM,Test,Training,Rqmt,PM,Benefits"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="double_chk" error="Please double check, maybe NOT iin Hydra List" sqref="A3:A1048576">
+      <formula1>"1FB ODC,Affinity Product,CS-Maintenance,OP Product,1FB Test,ODC:Falcon,Bleum"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -617,15 +1488,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:J15"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="57" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1014,34 +1889,34 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13">
-        <v>9011</v>
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1055,13 +1930,13 @@
         <v>26</v>
       </c>
       <c r="D14">
-        <v>9023</v>
+        <v>9011</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1078,22 +1953,22 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>9023</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1105,42 +1980,277 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17">
+        <v>9012</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
         <v>45</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
         <v>43</v>
       </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="double_chk" error="Please double check, maybe NOT iin Hydra List" sqref="B2:B23">
+      <formula1>"Admin&amp;HR,Quality,SCM,Test,Training,Rqmt,PM,Benefits"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="double_chk" error="Please double check, maybe NOT iin Hydra List" sqref="C2:C23">
+      <formula1>"Email,TAS,Resource Mgt,Reimburse,Tech. Improve,Technical,Manage change,Review Req.,Setup Env.,Build&amp;Install,Draft Spec.,Manage change,Meeting,Domain,QA Pcm,QA Audit,Paid Leave,Public Holidays,English"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="double_chk" error="Please double check, maybe NOT iin Hydra List" sqref="A2:A23">
+      <formula1>"1FB ODC,Affinity Product,CS-Maintenance,1FB Test,ODC:Falcon,Bleum"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1149,7 +2259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>